<commit_message>
saving for now, learning adders
</commit_message>
<xml_diff>
--- a/Labs/Lab3/Task2/TruthTable.xlsx
+++ b/Labs/Lab3/Task2/TruthTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital-Electronics-Fall-2023\Labs\Lab3\Task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5250785C-521F-4F58-9975-C7C413082897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99CA48EC-BD76-4DD8-A5AA-CAE94F30257B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="18">
   <si>
     <t>A</t>
   </si>
@@ -223,12 +224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,7 +236,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -249,11 +248,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,67 +338,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>352426</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7358B5B-1ED5-457C-8229-A8546C656A27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3324225" y="4972051"/>
-          <a:ext cx="457200" cy="714375"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>433387</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>90491</xdr:rowOff>
@@ -1252,67 +1192,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>366713</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>80969</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>157169</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="Rectangle: Rounded Corners 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{581580B2-6176-4B79-8677-6E5F5795A93A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="15232857" y="5179225"/>
-          <a:ext cx="457200" cy="928687"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -1676,6 +1555,1571 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A41BF61-ED50-4CA3-84DE-421B216AA3A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2695575" y="7458078"/>
+          <a:ext cx="842961" cy="1233487"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>366507</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>188781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295414</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>247484</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Arc 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C5663B-5660-4FE6-9C29-7FEB5CC1F7C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18823037" flipH="1">
+          <a:off x="3178159" y="6711629"/>
+          <a:ext cx="1011203" cy="538507"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 4614487"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>576692</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>564423</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>209769</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Arc 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382DBBCA-EA7E-43AF-BD2E-6720DA16F7DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="14343032" flipH="1">
+          <a:off x="803524" y="6468670"/>
+          <a:ext cx="1362867" cy="597331"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 4614487"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>51049</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>144069</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>194716</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>169900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Arc 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF1235C7-F14F-4CAC-90A2-E211EC979845}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="9070083" flipH="1">
+          <a:off x="660649" y="8145069"/>
+          <a:ext cx="1362867" cy="597331"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 4614487"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>557214</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>23818</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100018</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle: Rounded Corners 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E66DAA5-4FBD-4ADB-8973-CB2C6900C7E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2197894" y="6612738"/>
+          <a:ext cx="457200" cy="2519360"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33342</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>109542</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle: Rounded Corners 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07669DE6-8DAD-4E20-A5BD-0599DD21AA34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1802606" y="6655598"/>
+          <a:ext cx="457200" cy="928687"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297656</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>16674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>145256</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>183361</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle: Rounded Corners 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA94683-0F89-41CC-B700-4055B6435D7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3345656" y="6874674"/>
+          <a:ext cx="457200" cy="928687"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>567167</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>237551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>554898</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76418</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Arc 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4D7142D-D573-45DF-AA6D-9D22E0A1DB72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="13507730" flipH="1">
+          <a:off x="2622799" y="7859319"/>
+          <a:ext cx="1362867" cy="597331"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 4614487"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle: Rounded Corners 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A8411D9-0605-4B43-A244-5C556B4CCA44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7010400" y="7458078"/>
+          <a:ext cx="842961" cy="1233487"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>347666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle: Rounded Corners 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0996E071-F1E5-47FB-A6B9-C407D6BC8C76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5762625" y="6629403"/>
+          <a:ext cx="842961" cy="1233487"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>90917</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>37527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Arc 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CBB7925-69B2-48AA-8343-A65BD24784A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5693497" y="7541347"/>
+          <a:ext cx="972124" cy="1204483"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16199996"/>
+            <a:gd name="adj2" fmla="val 5319726"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>138544</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>276227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123827</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114303</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Arc 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD44643A-F548-49E7-97DC-4A729D32BBAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5736648" y="6641523"/>
+          <a:ext cx="981076" cy="1204483"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16199996"/>
+            <a:gd name="adj2" fmla="val 5319726"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>532972</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>81194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>157464</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80109</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Arc 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7C14D26-37DA-4FA5-879A-0468D6F58EAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10507527" flipH="1">
+          <a:off x="5409772" y="7320194"/>
+          <a:ext cx="843692" cy="760915"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16199996"/>
+            <a:gd name="adj2" fmla="val 5207605"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209122</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>443214</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137259</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Arc 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD33A66D-9D3A-4A34-AEA1-17AA1F5FC5A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="21336004" flipH="1">
+          <a:off x="7524322" y="7377344"/>
+          <a:ext cx="843692" cy="760915"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16199996"/>
+            <a:gd name="adj2" fmla="val 5207605"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Rectangle: Rounded Corners 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABFDE90-73BB-4C49-8D1E-B91518A2DD56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10582275" y="7458078"/>
+          <a:ext cx="842961" cy="1233487"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330994</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>130973</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle: Rounded Corners 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96907975-8129-4902-9E92-A3B546DA9FA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11913394" y="6772275"/>
+          <a:ext cx="457200" cy="1740698"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B35F4C41-35AD-4CB4-989F-8A02E472E365}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10406062" y="7091362"/>
+          <a:ext cx="352425" cy="857249"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104772</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rectangle: Rounded Corners 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63380273-B0F2-4E30-A3E8-CF4440A87498}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10834687" y="6986585"/>
+          <a:ext cx="352425" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rectangle: Rounded Corners 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43FDBF9E-280B-4A88-9FAF-16800E455284}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="11672887" y="6700837"/>
+          <a:ext cx="352425" cy="857249"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>174593</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13176</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2971134" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D6A2E08-FE16-7060-65E6-7C3CAC4A524E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="784193" y="5918676"/>
+          <a:ext cx="2971134" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S0=(B'+C')*(A+C')*(A+B'+D')*(A'+B+C)*(A'+D)*(B+D)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>193643</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>3651</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2270686" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD614C2-AAC3-5FBC-1317-0C24309A17F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5070443" y="5909151"/>
+          <a:ext cx="2270686" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S1=(B+D)*(A+C+D)*(A'+C+D')*(A+C'+D')</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>450818</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22701</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2707408" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="TextBox 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5CF4AE8-8B20-4BEE-A28E-D78DF7DE8EE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8985218" y="5928201"/>
+          <a:ext cx="2707408" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S2=(A+C+D)*(B'+C+D')*(A+C'+D')*(A+B')*(A'+B)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>60293</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>32226</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2884379" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="TextBox 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A11A315-935B-4639-B644-59BA15624949}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13471493" y="6128226"/>
+          <a:ext cx="2884379" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S3=(A'+C)*(A+B+D)*(B+C'+D')*(B'+C+D')*(B'+C'+D)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>307943</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>13176</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2367251" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="TextBox 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2789A41-1D93-4912-812F-FE4252254083}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="307943" y="8776176"/>
+          <a:ext cx="2367251" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S4=(B+D)*(A'+B')*(C'+D)*(A'+C')*(A+B+C)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>317468</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>13176</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1763368" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="TextBox 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037F9B3C-DB5D-45B8-85B2-2B32DBCC53A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5194268" y="8585676"/>
+          <a:ext cx="1763368" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S5=(A+C)*(A'+C')*(B'+D)*(B+C)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>517493</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>13176</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2550314" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="TextBox 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9056AA02-819F-471C-82E0-1D0128EA9170}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9051893" y="8585676"/>
+          <a:ext cx="2550314" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>S6=(C'+D)*(A'+B)*(A'+D')*(A+B'+C)*(A+B+C')</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1942,654 +3386,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1</v>
-      </c>
-      <c r="L4" s="9">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>0</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
-      <c r="L5" s="9">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>0</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>0</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1</v>
-      </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
-      <c r="L9" s="9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8">
-        <v>1</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>1</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>1</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>1</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="9">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
-        <v>0</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0</v>
-      </c>
-      <c r="K15" s="8">
-        <v>1</v>
-      </c>
-      <c r="L15" s="9">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="K16" s="8">
-        <v>0</v>
-      </c>
-      <c r="L16" s="9">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-      <c r="C17" s="11">
-        <v>1</v>
-      </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="10">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="11">
-        <v>1</v>
-      </c>
-      <c r="J17" s="11">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C19" s="17" t="s">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="J19" s="17" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="J19" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="Q19" s="17" t="s">
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="Q19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="X19" s="17" t="s">
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="X19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="Y19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="17"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
@@ -2603,23 +4029,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -2628,16 +4054,16 @@
       <c r="I21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="K21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="16" t="s">
+      <c r="M21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -2646,16 +4072,16 @@
       <c r="P21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q21" s="16" t="s">
+      <c r="Q21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="R21" s="16" t="s">
+      <c r="R21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="S21" s="16" t="s">
+      <c r="S21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T21" s="16" t="s">
+      <c r="T21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="V21" s="1" t="s">
@@ -2664,321 +4090,544 @@
       <c r="W21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X21" s="16" t="s">
+      <c r="X21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Y21" s="16" t="s">
+      <c r="Y21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Z21" s="16" t="s">
+      <c r="Z21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AA21" s="16" t="s">
+      <c r="AA21" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="15">
         <v>0</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13">
         <v>0</v>
       </c>
       <c r="F22" s="15">
         <v>0</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="18">
-        <v>0</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-      <c r="M22" s="18">
-        <v>0</v>
-      </c>
-      <c r="P22" s="16" t="s">
+      <c r="J22" s="15">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="15">
+        <v>0</v>
+      </c>
+      <c r="P22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q22" s="19">
-        <v>0</v>
-      </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19">
-        <v>0</v>
-      </c>
-      <c r="T22" s="19"/>
-      <c r="W22" s="16" t="s">
+      <c r="Q22" s="13">
+        <v>0</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13">
+        <v>0</v>
+      </c>
+      <c r="T22" s="13"/>
+      <c r="W22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="X22" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="19">
+      <c r="X22" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="15">
-        <v>0</v>
-      </c>
-      <c r="I23" s="16" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="15">
-        <v>0</v>
-      </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15">
-        <v>0</v>
-      </c>
-      <c r="M23" s="15"/>
-      <c r="P23" s="16" t="s">
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="P23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q23" s="19">
-        <v>0</v>
-      </c>
-      <c r="R23" s="15">
-        <v>0</v>
-      </c>
-      <c r="S23" s="19">
-        <v>0</v>
-      </c>
-      <c r="T23" s="19">
-        <v>0</v>
-      </c>
-      <c r="W23" s="16" t="s">
+      <c r="Q23" s="13">
+        <v>0</v>
+      </c>
+      <c r="R23" s="13">
+        <v>0</v>
+      </c>
+      <c r="S23" s="13">
+        <v>0</v>
+      </c>
+      <c r="T23" s="13">
+        <v>0</v>
+      </c>
+      <c r="W23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19">
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="15">
-        <v>0</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15">
-        <v>0</v>
-      </c>
-      <c r="F24" s="15">
-        <v>0</v>
-      </c>
-      <c r="I24" s="16" t="s">
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15">
-        <v>0</v>
-      </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="P24" s="16" t="s">
+      <c r="J24" s="13"/>
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="P24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19">
-        <v>0</v>
-      </c>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="W24" s="16" t="s">
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13">
+        <v>0</v>
+      </c>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="W24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="X24" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19">
+      <c r="X24" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="15">
         <v>0</v>
       </c>
-      <c r="D25" s="15">
-        <v>0</v>
-      </c>
-      <c r="E25" s="15"/>
+      <c r="D25" s="13">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13"/>
       <c r="F25" s="15">
         <v>0</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="18">
-        <v>0</v>
-      </c>
-      <c r="K25" s="15">
-        <v>0</v>
-      </c>
-      <c r="L25" s="15"/>
-      <c r="M25" s="18">
-        <v>0</v>
-      </c>
-      <c r="P25" s="16" t="s">
+      <c r="J25" s="15">
+        <v>0</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13"/>
+      <c r="M25" s="15">
+        <v>0</v>
+      </c>
+      <c r="P25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="19">
-        <v>0</v>
-      </c>
-      <c r="R25" s="19">
-        <v>0</v>
-      </c>
-      <c r="S25" s="19">
-        <v>0</v>
-      </c>
-      <c r="T25" s="19">
-        <v>0</v>
-      </c>
-      <c r="W25" s="16" t="s">
+      <c r="Q25" s="13">
+        <v>0</v>
+      </c>
+      <c r="R25" s="13">
+        <v>0</v>
+      </c>
+      <c r="S25" s="13">
+        <v>0</v>
+      </c>
+      <c r="T25" s="13">
+        <v>0</v>
+      </c>
+      <c r="W25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="X25" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="19"/>
+      <c r="X25" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="13"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="J28" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="Q28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="30" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="31" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+    <row r="31" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="19">
-        <v>0</v>
-      </c>
-      <c r="D31" s="19">
-        <v>0</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19">
+      <c r="C31" s="13">
+        <v>0</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13">
+        <v>0</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="13">
+        <v>0</v>
+      </c>
+      <c r="K31" s="13">
+        <v>0</v>
+      </c>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="P31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13">
+        <v>0</v>
+      </c>
+      <c r="T31" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+    <row r="32" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="19">
-        <v>0</v>
-      </c>
-      <c r="F32" s="19"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
+        <v>0</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="13">
+        <v>0</v>
+      </c>
+      <c r="K32" s="13">
+        <v>0</v>
+      </c>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13">
+        <v>0</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q32" s="13">
+        <v>0</v>
+      </c>
+      <c r="R32" s="13">
+        <v>0</v>
+      </c>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
+    <row r="33" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="19">
-        <v>0</v>
-      </c>
-      <c r="D33" s="19">
-        <v>0</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19">
+      <c r="C33" s="13">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0</v>
+      </c>
+      <c r="F33" s="13">
+        <v>0</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="13">
+        <v>0</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13">
+        <v>0</v>
+      </c>
+      <c r="M33" s="13">
+        <v>0</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13">
+        <v>0</v>
+      </c>
+      <c r="S33" s="13">
+        <v>0</v>
+      </c>
+      <c r="T33" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
+    <row r="34" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="19">
-        <v>0</v>
-      </c>
-      <c r="D34" s="19">
-        <v>0</v>
-      </c>
-      <c r="E34" s="19">
-        <v>0</v>
-      </c>
-      <c r="F34" s="19"/>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13">
+        <v>0</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0</v>
+      </c>
+      <c r="K34" s="13">
+        <v>0</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q34" s="13">
+        <v>0</v>
+      </c>
+      <c r="R34" s="13">
+        <v>0</v>
+      </c>
+      <c r="S34" s="13">
+        <v>0</v>
+      </c>
+      <c r="T34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="H36:N36"/>
+    <mergeCell ref="O36:T36"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="J19:M19"/>
     <mergeCell ref="Q19:T19"/>
     <mergeCell ref="X19:AA19"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="Q28:T28"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:N27"/>
+    <mergeCell ref="O27:U27"/>
+    <mergeCell ref="V28:AB28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>